<commit_message>
shorthand man changed to mfg
</commit_message>
<xml_diff>
--- a/ShortHands.xlsx
+++ b/ShortHands.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akitt/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akitt/Code/AM-CDM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE86B97-5480-0A47-A2B1-316BC70B7150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F5579F-6542-DD49-AFDE-B6AAE088FC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" xr2:uid="{D075A580-C83A-6248-82D1-7622755D1633}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="18000" xr2:uid="{D075A580-C83A-6248-82D1-7622755D1633}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -309,12 +309,6 @@
     <t>AugmentedSourceModel</t>
   </si>
   <si>
-    <t>manProcess</t>
-  </si>
-  <si>
-    <t>manSpec</t>
-  </si>
-  <si>
     <t>partSpec</t>
   </si>
   <si>
@@ -514,6 +508,12 @@
   </si>
   <si>
     <t>buildEnvironmentControl</t>
+  </si>
+  <si>
+    <t>mfgProcess</t>
+  </si>
+  <si>
+    <t>mfgSpec</t>
   </si>
 </sst>
 </file>
@@ -922,7 +922,7 @@
   <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -970,7 +970,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -989,7 +989,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1151,7 +1151,7 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1228,7 +1228,7 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1239,7 +1239,7 @@
         <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1250,7 +1250,7 @@
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1269,7 +1269,7 @@
         <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1296,7 +1296,7 @@
         <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1323,7 +1323,7 @@
         <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1334,7 +1334,7 @@
         <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1345,7 +1345,7 @@
         <v>61</v>
       </c>
       <c r="C40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1356,7 +1356,7 @@
         <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1367,7 +1367,7 @@
         <v>63</v>
       </c>
       <c r="C42" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1378,7 +1378,7 @@
         <v>64</v>
       </c>
       <c r="C43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1397,7 +1397,7 @@
         <v>66</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1408,7 +1408,7 @@
         <v>67</v>
       </c>
       <c r="C46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1419,86 +1419,86 @@
         <v>68</v>
       </c>
       <c r="C47" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C48" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" t="s">
         <v>95</v>
-      </c>
-      <c r="B49" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B51" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C51" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B53" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C53" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B54" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C54" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C55" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1520,7 +1520,7 @@
         <v>71</v>
       </c>
       <c r="C57" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1531,7 +1531,7 @@
         <v>72</v>
       </c>
       <c r="C58" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1560,210 +1560,210 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B62" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C62" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" t="s">
         <v>109</v>
       </c>
-      <c r="B63" t="s">
-        <v>111</v>
-      </c>
       <c r="C63" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B64" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C64" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B65" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C65" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B66" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C66" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B67" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C67" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B68" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C68" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B69" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C69" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B70" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C70" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B71" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C71" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B72" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C72" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B73" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B74" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B75" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B76" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B77" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C77" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B78" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C78" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B79" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C79" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B80" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C80" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B81" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C81" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>